<commit_message>
merge file in Danh folder and improve code detect arrhythmia by HRV
can't detect signal which have problem with PR ratio
add code arrhythmia detection
</commit_message>
<xml_diff>
--- a/data analysis/Arrhythmia data analysis.xlsx
+++ b/data analysis/Arrhythmia data analysis.xlsx
@@ -81,10 +81,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -104,15 +104,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -127,6 +141,29 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -136,14 +173,15 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -157,11 +195,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -180,9 +218,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -190,36 +227,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,15 +246,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,7 +268,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,25 +358,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -316,13 +388,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -340,7 +418,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,103 +442,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -622,6 +616,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -637,26 +640,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -685,6 +679,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -692,21 +701,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -724,7 +718,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -742,134 +736,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -951,15 +945,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -970,15 +955,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1307,7 +1283,7 @@
   <dimension ref="A1:XFD102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A44" sqref="A44:L45"/>
     </sheetView>
@@ -2989,7 +2965,7 @@
       <c r="F48" s="9"/>
       <c r="G48" s="7"/>
       <c r="H48" s="9"/>
-      <c r="I48" s="32">
+      <c r="I48" s="29">
         <v>1.9567</v>
       </c>
       <c r="J48" s="9">
@@ -3017,7 +2993,7 @@
       <c r="F49" s="9"/>
       <c r="G49" s="7"/>
       <c r="H49" s="9"/>
-      <c r="I49" s="32">
+      <c r="I49" s="29">
         <v>17.3363</v>
       </c>
       <c r="J49" s="9">
@@ -3045,7 +3021,7 @@
       <c r="F50" s="9"/>
       <c r="G50" s="7"/>
       <c r="H50" s="9"/>
-      <c r="I50" s="32">
+      <c r="I50" s="29">
         <v>21.6949</v>
       </c>
       <c r="J50" s="9">
@@ -3073,7 +3049,7 @@
       <c r="F51" s="9"/>
       <c r="G51" s="7"/>
       <c r="H51" s="9"/>
-      <c r="I51" s="32">
+      <c r="I51" s="29">
         <v>19.2481203007519</v>
       </c>
       <c r="J51" s="9">
@@ -3101,7 +3077,7 @@
       <c r="F52" s="9"/>
       <c r="G52" s="7"/>
       <c r="H52" s="9"/>
-      <c r="I52" s="32">
+      <c r="I52" s="29">
         <v>7.74193548387097</v>
       </c>
       <c r="J52" s="9">
@@ -3157,7 +3133,7 @@
       <c r="F54" s="9"/>
       <c r="G54" s="7"/>
       <c r="H54" s="9"/>
-      <c r="I54" s="32">
+      <c r="I54" s="29">
         <v>4.15809420682187</v>
       </c>
       <c r="J54" s="9">
@@ -3213,7 +3189,7 @@
       <c r="F56" s="9"/>
       <c r="G56" s="7"/>
       <c r="H56" s="9"/>
-      <c r="I56" s="32">
+      <c r="I56" s="29">
         <v>8.73720136518771</v>
       </c>
       <c r="J56" s="9">
@@ -3241,7 +3217,7 @@
       <c r="F57" s="9"/>
       <c r="G57" s="7"/>
       <c r="H57" s="9"/>
-      <c r="I57" s="32">
+      <c r="I57" s="29">
         <v>8.57142857142857</v>
       </c>
       <c r="J57" s="9">
@@ -3269,7 +3245,7 @@
       <c r="F58" s="9"/>
       <c r="G58" s="7"/>
       <c r="H58" s="9"/>
-      <c r="I58" s="32">
+      <c r="I58" s="29">
         <v>0.336546888694128</v>
       </c>
       <c r="J58" s="9">
@@ -3297,7 +3273,7 @@
       <c r="F59" s="9"/>
       <c r="G59" s="7"/>
       <c r="H59" s="9"/>
-      <c r="I59" s="32">
+      <c r="I59" s="29">
         <v>0.618457078434531</v>
       </c>
       <c r="J59" s="9">
@@ -3325,7 +3301,7 @@
       <c r="F60" s="12"/>
       <c r="G60" s="10"/>
       <c r="H60" s="12"/>
-      <c r="I60" s="33">
+      <c r="I60" s="30">
         <v>5.73991031390135</v>
       </c>
       <c r="J60" s="12">
@@ -3343,28 +3319,28 @@
         <v>13</v>
       </c>
       <c r="B61" s="26"/>
-      <c r="C61" s="27"/>
-      <c r="D61" s="28">
+      <c r="C61" s="23"/>
+      <c r="D61" s="24">
         <f t="shared" ref="D61:L61" si="1">AVERAGE(D47:D60)</f>
         <v>0.524632343225701</v>
       </c>
-      <c r="E61" s="27"/>
-      <c r="F61" s="28"/>
-      <c r="G61" s="29"/>
-      <c r="H61" s="29"/>
-      <c r="I61" s="27">
+      <c r="E61" s="23"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="22"/>
+      <c r="I61" s="23">
         <f t="shared" si="1"/>
         <v>14.8460606042747</v>
       </c>
-      <c r="J61" s="28">
+      <c r="J61" s="24">
         <f t="shared" si="1"/>
         <v>172.238378738854</v>
       </c>
-      <c r="K61" s="29">
+      <c r="K61" s="22">
         <f t="shared" si="1"/>
         <v>22.3243448708806</v>
       </c>
-      <c r="L61" s="28">
+      <c r="L61" s="24">
         <f t="shared" si="1"/>
         <v>16.1692071586742</v>
       </c>
@@ -3376,31 +3352,31 @@
       <c r="A63" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B63" s="30"/>
-      <c r="C63" s="30"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="30"/>
-      <c r="G63" s="30"/>
-      <c r="H63" s="30"/>
-      <c r="I63" s="30"/>
-      <c r="J63" s="30"/>
-      <c r="K63" s="30"/>
-      <c r="L63" s="30"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="27"/>
+      <c r="I63" s="27"/>
+      <c r="J63" s="27"/>
+      <c r="K63" s="27"/>
+      <c r="L63" s="27"/>
     </row>
     <row r="64" customFormat="1" ht="37" customHeight="1" spans="1:12">
-      <c r="A64" s="31"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
-      <c r="G64" s="30"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="30"/>
-      <c r="J64" s="30"/>
-      <c r="K64" s="30"/>
-      <c r="L64" s="30"/>
+      <c r="A64" s="28"/>
+      <c r="B64" s="27"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="27"/>
+      <c r="G64" s="27"/>
+      <c r="H64" s="27"/>
+      <c r="I64" s="27"/>
+      <c r="J64" s="27"/>
+      <c r="K64" s="27"/>
+      <c r="L64" s="27"/>
     </row>
     <row r="65" s="1" customFormat="1" ht="15.75" spans="1:1">
       <c r="A65" s="19"/>
@@ -3409,7 +3385,7 @@
       <c r="A66" s="22">
         <v>103</v>
       </c>
-      <c r="B66" s="34" t="s">
+      <c r="B66" s="23" t="s">
         <v>17</v>
       </c>
       <c r="C66" s="23">
@@ -3447,7 +3423,7 @@
       <c r="A67" s="7">
         <v>104</v>
       </c>
-      <c r="B67" s="35" t="s">
+      <c r="B67" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C67" s="8">
@@ -3485,7 +3461,7 @@
       <c r="A68" s="7">
         <v>105</v>
       </c>
-      <c r="B68" s="35" t="s">
+      <c r="B68" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C68" s="8">
@@ -3523,7 +3499,7 @@
       <c r="A69" s="7">
         <v>106</v>
       </c>
-      <c r="B69" s="35" t="s">
+      <c r="B69" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C69" s="8">
@@ -3561,7 +3537,7 @@
       <c r="A70" s="7">
         <v>112</v>
       </c>
-      <c r="B70" s="35" t="s">
+      <c r="B70" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C70" s="8">
@@ -3599,7 +3575,7 @@
       <c r="A71" s="7">
         <v>113</v>
       </c>
-      <c r="B71" s="35" t="s">
+      <c r="B71" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C71" s="8">
@@ -3637,7 +3613,7 @@
       <c r="A72" s="7">
         <v>118</v>
       </c>
-      <c r="B72" s="35" t="s">
+      <c r="B72" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C72" s="8">
@@ -3675,7 +3651,7 @@
       <c r="A73" s="7">
         <v>121</v>
       </c>
-      <c r="B73" s="35" t="s">
+      <c r="B73" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C73" s="8">
@@ -3713,7 +3689,7 @@
       <c r="A74" s="7">
         <v>129</v>
       </c>
-      <c r="B74" s="35" t="s">
+      <c r="B74" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C74" s="8">
@@ -3751,7 +3727,7 @@
       <c r="A75" s="7">
         <v>133</v>
       </c>
-      <c r="B75" s="35" t="s">
+      <c r="B75" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C75" s="8">
@@ -3789,7 +3765,7 @@
       <c r="A76" s="7">
         <v>136</v>
       </c>
-      <c r="B76" s="35" t="s">
+      <c r="B76" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C76" s="8">
@@ -3827,7 +3803,7 @@
       <c r="A77" s="7">
         <v>139</v>
       </c>
-      <c r="B77" s="35" t="s">
+      <c r="B77" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C77" s="8">
@@ -3865,7 +3841,7 @@
       <c r="A78" s="7">
         <v>154</v>
       </c>
-      <c r="B78" s="35" t="s">
+      <c r="B78" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C78" s="8">
@@ -3903,7 +3879,7 @@
       <c r="A79" s="7">
         <v>161</v>
       </c>
-      <c r="B79" s="35" t="s">
+      <c r="B79" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C79" s="8">
@@ -3941,7 +3917,7 @@
       <c r="A80" s="7">
         <v>162</v>
       </c>
-      <c r="B80" s="35" t="s">
+      <c r="B80" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C80" s="8">
@@ -3979,7 +3955,7 @@
       <c r="A81" s="7">
         <v>163</v>
       </c>
-      <c r="B81" s="35" t="s">
+      <c r="B81" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C81" s="8">
@@ -4017,7 +3993,7 @@
       <c r="A82" s="7">
         <v>170</v>
       </c>
-      <c r="B82" s="35" t="s">
+      <c r="B82" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C82" s="8">
@@ -4055,7 +4031,7 @@
       <c r="A83" s="7">
         <v>105</v>
       </c>
-      <c r="B83" s="35" t="s">
+      <c r="B83" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C83" s="8">
@@ -4093,7 +4069,7 @@
       <c r="A84" s="7">
         <v>108</v>
       </c>
-      <c r="B84" s="35" t="s">
+      <c r="B84" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C84" s="8">
@@ -4131,7 +4107,7 @@
       <c r="A85" s="7">
         <v>112</v>
       </c>
-      <c r="B85" s="35" t="s">
+      <c r="B85" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C85" s="8">
@@ -4169,7 +4145,7 @@
       <c r="A86" s="7">
         <v>115</v>
       </c>
-      <c r="B86" s="35" t="s">
+      <c r="B86" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C86" s="8">
@@ -4207,7 +4183,7 @@
       <c r="A87" s="7">
         <v>123</v>
       </c>
-      <c r="B87" s="35" t="s">
+      <c r="B87" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C87" s="8">
@@ -4245,7 +4221,7 @@
       <c r="A88" s="7">
         <v>129</v>
       </c>
-      <c r="B88" s="35" t="s">
+      <c r="B88" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C88" s="8">
@@ -4283,7 +4259,7 @@
       <c r="A89" s="7">
         <v>133</v>
       </c>
-      <c r="B89" s="35" t="s">
+      <c r="B89" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C89" s="8">
@@ -4321,7 +4297,7 @@
       <c r="A90" s="7">
         <v>147</v>
       </c>
-      <c r="B90" s="35" t="s">
+      <c r="B90" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C90" s="8">
@@ -4359,7 +4335,7 @@
       <c r="A91" s="7">
         <v>154</v>
       </c>
-      <c r="B91" s="35" t="s">
+      <c r="B91" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C91" s="8">
@@ -4397,7 +4373,7 @@
       <c r="A92" s="7">
         <v>104</v>
       </c>
-      <c r="B92" s="35" t="s">
+      <c r="B92" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C92" s="8">
@@ -4435,7 +4411,7 @@
       <c r="A93" s="7">
         <v>112</v>
       </c>
-      <c r="B93" s="35" t="s">
+      <c r="B93" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C93" s="8">
@@ -4473,7 +4449,7 @@
       <c r="A94" s="7">
         <v>118</v>
       </c>
-      <c r="B94" s="35" t="s">
+      <c r="B94" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C94" s="8">
@@ -4511,7 +4487,7 @@
       <c r="A95" s="7">
         <v>122</v>
       </c>
-      <c r="B95" s="35" t="s">
+      <c r="B95" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C95" s="8">
@@ -4549,7 +4525,7 @@
       <c r="A96" s="7">
         <v>154</v>
       </c>
-      <c r="B96" s="35" t="s">
+      <c r="B96" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C96" s="8">
@@ -4587,7 +4563,7 @@
       <c r="A97" s="7">
         <v>161</v>
       </c>
-      <c r="B97" s="35" t="s">
+      <c r="B97" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C97" s="8">
@@ -4625,7 +4601,7 @@
       <c r="A98" s="7">
         <v>612</v>
       </c>
-      <c r="B98" s="35" t="s">
+      <c r="B98" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C98" s="8">
@@ -4663,7 +4639,7 @@
       <c r="A99" s="7">
         <v>801</v>
       </c>
-      <c r="B99" s="35" t="s">
+      <c r="B99" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C99" s="8">
@@ -4701,7 +4677,7 @@
       <c r="A100" s="10">
         <v>808</v>
       </c>
-      <c r="B100" s="36" t="s">
+      <c r="B100" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C100" s="11">
@@ -4736,10 +4712,10 @@
       </c>
     </row>
     <row r="101" ht="15.75" spans="1:12">
-      <c r="A101" s="37" t="s">
+      <c r="A101" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B101" s="38"/>
+      <c r="B101" s="32"/>
       <c r="C101" s="11">
         <f>AVERAGE(C66:C100)</f>
         <v>0.652822354475927</v>
@@ -4782,16 +4758,16 @@
       </c>
     </row>
     <row r="102" spans="5:10">
-      <c r="E102" s="39">
+      <c r="E102" s="33">
         <f>AVERAGE(E101:F101)</f>
         <v>82.6913658869488</v>
       </c>
-      <c r="F102" s="39"/>
-      <c r="I102" s="39">
+      <c r="F102" s="33"/>
+      <c r="I102" s="33">
         <f>AVERAGE(I101:J101)</f>
         <v>104.129811808066</v>
       </c>
-      <c r="J102" s="39"/>
+      <c r="J102" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>